<commit_message>
Modification in README.md file
</commit_message>
<xml_diff>
--- a/Results/CSI_1_results.xlsx
+++ b/Results/CSI_1_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avijitmajhi/Desktop/radar_nowcasting/Results/backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Geosciences_Project\Nowcasting_OF\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70D33F7-2732-3C41-91E1-9009C706A9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B202279-28B5-429D-A3D8-DBDA320A5A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LK_persistence" sheetId="7" r:id="rId1"/>
@@ -25,13 +25,15 @@
     <sheet name="proesmans_extrapolation" sheetId="11" r:id="rId10"/>
     <sheet name="proesmans_sprog" sheetId="12" r:id="rId11"/>
     <sheet name="proesmans_anvil" sheetId="13" r:id="rId12"/>
+    <sheet name="VET_persistence" sheetId="14" r:id="rId13"/>
+    <sheet name="VET_extrapolation" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="19">
   <si>
     <t>Event</t>
   </si>
@@ -94,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +109,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,9 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -457,9 +467,9 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -505,7 +515,7 @@
         <v>7.7750884338902898E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -528,7 +538,7 @@
         <v>0.15808902178187839</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -551,7 +561,7 @@
         <v>7.0571704114618605E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -574,7 +584,7 @@
         <v>4.5460779173834343E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -597,7 +607,7 @@
         <v>4.7675201910522033E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -620,7 +630,7 @@
         <v>1.9320874579757969E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -643,7 +653,7 @@
         <v>2.9460959935557269E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -666,7 +676,7 @@
         <v>0.1021658779432687</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -689,7 +699,7 @@
         <v>8.9785009060016033E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -712,7 +722,7 @@
         <v>6.8258077972422601E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -735,7 +745,7 @@
         <v>6.0182814811351293E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -771,9 +781,9 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -819,7 +829,7 @@
         <v>8.1852047241299006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -842,7 +852,7 @@
         <v>0.1099162771445955</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -865,7 +875,7 @@
         <v>3.5104806941419271E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -888,7 +898,7 @@
         <v>7.2804813360333037E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -911,7 +921,7 @@
         <v>3.4145130395470492E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -934,7 +944,7 @@
         <v>7.1844795521068205E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -957,7 +967,7 @@
         <v>4.9398275090017367E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -980,7 +990,7 @@
         <v>5.758962650075513E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1013,7 @@
         <v>3.8837697697260462E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>1.6144382174115821E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1059,7 @@
         <v>7.2749667677109955E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1085,9 +1095,9 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1133,7 +1143,7 @@
         <v>0.1169341232493256</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1156,7 +1166,7 @@
         <v>0.15099937394611651</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>4.1423848494914053E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1202,7 +1212,7 @@
         <v>0.10197848523467171</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>3.7010756554225012E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1248,7 +1258,7 @@
         <v>9.1822658044343086E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>6.6286128778383788E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1294,7 +1304,7 @@
         <v>5.3413951175625543E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>6.6711317682271024E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1340,7 +1350,7 @@
         <v>2.3884306841639551E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>7.7284500709372636E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1399,9 +1409,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1457,7 @@
         <v>8.82725165238962E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1480,7 @@
         <v>0.1108120319474033</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1493,7 +1503,7 @@
         <v>3.7029114975777558E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1516,7 +1526,7 @@
         <v>6.6713566988717207E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1539,7 +1549,7 @@
         <v>3.5621464202108599E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1562,7 +1572,7 @@
         <v>7.2915012255630698E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1585,7 +1595,7 @@
         <v>5.2315014022578321E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1608,7 +1618,7 @@
         <v>6.1536205208376431E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1641,7 @@
         <v>3.8866726751149133E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1654,7 +1664,7 @@
         <v>1.8248155196988951E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1687,7 @@
         <v>8.126931745381033E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1702,6 +1712,630 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5727EB-4F5F-4BBA-AD38-0E35DB082C89}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.34847078528093761</v>
+      </c>
+      <c r="C2">
+        <v>0.20657729728399099</v>
+      </c>
+      <c r="D2">
+        <v>0.14283322642220889</v>
+      </c>
+      <c r="E2">
+        <v>0.10449376677107799</v>
+      </c>
+      <c r="F2">
+        <v>8.0780644502555149E-2</v>
+      </c>
+      <c r="G2">
+        <v>6.7002638535033729E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.42973772801780902</v>
+      </c>
+      <c r="C3">
+        <v>0.267317091131477</v>
+      </c>
+      <c r="D3">
+        <v>0.19420543974774271</v>
+      </c>
+      <c r="E3">
+        <v>0.14615323284923931</v>
+      </c>
+      <c r="F3">
+        <v>0.10863080162755009</v>
+      </c>
+      <c r="G3">
+        <v>7.7750884338902898E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>7.3506261782311622E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.116610517749255E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.026140816005644E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.697905299759264E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.0935923285330751E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.5460779173834343E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.40653954632564759</v>
+      </c>
+      <c r="C5">
+        <v>0.25934343340647331</v>
+      </c>
+      <c r="D5">
+        <v>0.1864329149978555</v>
+      </c>
+      <c r="E5">
+        <v>0.13548552225614749</v>
+      </c>
+      <c r="F5">
+        <v>9.6970336628080703E-2</v>
+      </c>
+      <c r="G5">
+        <v>6.8258077972422601E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>9.7807121511178097E-2</v>
+      </c>
+      <c r="C6">
+        <v>6.3358229707456887E-2</v>
+      </c>
+      <c r="D6">
+        <v>5.5416255175492632E-2</v>
+      </c>
+      <c r="E6">
+        <v>5.1360746133378751E-2</v>
+      </c>
+      <c r="F6">
+        <v>4.3632130485364892E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.9320874579757969E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>0.47796097952526001</v>
+      </c>
+      <c r="C7">
+        <v>0.28524806061663133</v>
+      </c>
+      <c r="D7">
+        <v>0.18847598728427589</v>
+      </c>
+      <c r="E7">
+        <v>0.13118208993216729</v>
+      </c>
+      <c r="F7">
+        <v>8.9678030164244221E-2</v>
+      </c>
+      <c r="G7">
+        <v>6.0182814811351293E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.25306525044456413</v>
+      </c>
+      <c r="C8">
+        <v>0.16122256394848511</v>
+      </c>
+      <c r="D8">
+        <v>0.12636935219907469</v>
+      </c>
+      <c r="E8">
+        <v>9.7234758097743401E-2</v>
+      </c>
+      <c r="F8">
+        <v>9.1992835936770684E-2</v>
+      </c>
+      <c r="G8">
+        <v>7.0571704114618605E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0.22571130028517769</v>
+      </c>
+      <c r="C9">
+        <v>0.10397584918959039</v>
+      </c>
+      <c r="D9">
+        <v>0.1012622835114096</v>
+      </c>
+      <c r="E9">
+        <v>0.1141565370792836</v>
+      </c>
+      <c r="F9">
+        <v>0.124133718072986</v>
+      </c>
+      <c r="G9">
+        <v>0.1021658779432687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.39232696788164839</v>
+      </c>
+      <c r="C10">
+        <v>0.21706468613028129</v>
+      </c>
+      <c r="D10">
+        <v>0.13353450666139671</v>
+      </c>
+      <c r="E10">
+        <v>8.3044379565437976E-2</v>
+      </c>
+      <c r="F10">
+        <v>6.3112406247336911E-2</v>
+      </c>
+      <c r="G10">
+        <v>4.7675201910522033E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>6.013213258964837E-2</v>
+      </c>
+      <c r="C11">
+        <v>1.8439261400206991E-2</v>
+      </c>
+      <c r="D11">
+        <v>2.4585141814057219E-2</v>
+      </c>
+      <c r="E11">
+        <v>3.0108384011536211E-2</v>
+      </c>
+      <c r="F11">
+        <v>3.096864391086683E-2</v>
+      </c>
+      <c r="G11">
+        <v>2.9460959935557269E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.37260787625432867</v>
+      </c>
+      <c r="C12">
+        <v>0.24412611647619581</v>
+      </c>
+      <c r="D12">
+        <v>0.1701242340861836</v>
+      </c>
+      <c r="E12">
+        <v>0.1314104578169023</v>
+      </c>
+      <c r="F12">
+        <v>0.1077418318120619</v>
+      </c>
+      <c r="G12">
+        <v>8.9785009060016033E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0.45207980570316991</v>
+      </c>
+      <c r="C13">
+        <v>0.30822964513480289</v>
+      </c>
+      <c r="D13">
+        <v>0.2381942629473624</v>
+      </c>
+      <c r="E13">
+        <v>0.19794567147584791</v>
+      </c>
+      <c r="F13">
+        <v>0.17471299677294741</v>
+      </c>
+      <c r="G13">
+        <v>0.15808902178187839</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92713F65-47E8-4579-8FB5-65F298BF647F}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.54305775985406668</v>
+      </c>
+      <c r="C2">
+        <v>0.37957508616374702</v>
+      </c>
+      <c r="D2">
+        <v>0.28796804287545841</v>
+      </c>
+      <c r="E2">
+        <v>0.22922923183821259</v>
+      </c>
+      <c r="F2">
+        <v>0.1869500041466215</v>
+      </c>
+      <c r="G2">
+        <v>0.15380936419628571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.64834896438464429</v>
+      </c>
+      <c r="C3">
+        <v>0.49934293669837881</v>
+      </c>
+      <c r="D3">
+        <v>0.40661988016707601</v>
+      </c>
+      <c r="E3">
+        <v>0.33760537887481329</v>
+      </c>
+      <c r="F3">
+        <v>0.27550397585578412</v>
+      </c>
+      <c r="G3">
+        <v>0.2210150843117773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>5.4545188263365067E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.8054905652850121E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.2757172262503849E-2</v>
+      </c>
+      <c r="E4">
+        <v>8.7622217476931979E-3</v>
+      </c>
+      <c r="F4">
+        <v>1.266875486398447E-2</v>
+      </c>
+      <c r="G4">
+        <v>5.0548433379843669E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.55399305507806029</v>
+      </c>
+      <c r="C5">
+        <v>0.37286585385665738</v>
+      </c>
+      <c r="D5">
+        <v>0.26859426514967338</v>
+      </c>
+      <c r="E5">
+        <v>0.20508435560008889</v>
+      </c>
+      <c r="F5">
+        <v>0.16316414996814341</v>
+      </c>
+      <c r="G5">
+        <v>0.13349414280082211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0.17955047596842921</v>
+      </c>
+      <c r="C6">
+        <v>8.1450247481258869E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.7093858319336183E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.0452783504902209E-2</v>
+      </c>
+      <c r="F6">
+        <v>7.4212324812973031E-3</v>
+      </c>
+      <c r="G6">
+        <v>9.5825532030025646E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>0.55423143957345822</v>
+      </c>
+      <c r="C7">
+        <v>0.35495217450879302</v>
+      </c>
+      <c r="D7">
+        <v>0.24771327833511661</v>
+      </c>
+      <c r="E7">
+        <v>0.1845702414959117</v>
+      </c>
+      <c r="F7">
+        <v>0.1412584282779879</v>
+      </c>
+      <c r="G7">
+        <v>0.10982556760443341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.49009946341615801</v>
+      </c>
+      <c r="C8">
+        <v>0.32214717092039402</v>
+      </c>
+      <c r="D8">
+        <v>0.22669509264979809</v>
+      </c>
+      <c r="E8">
+        <v>0.16158330651940311</v>
+      </c>
+      <c r="F8">
+        <v>0.1197440860151482</v>
+      </c>
+      <c r="G8">
+        <v>8.8538936683520156E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0.40460576621925071</v>
+      </c>
+      <c r="C9">
+        <v>0.2241751017540399</v>
+      </c>
+      <c r="D9">
+        <v>0.1213529991790033</v>
+      </c>
+      <c r="E9">
+        <v>6.8198268881454277E-2</v>
+      </c>
+      <c r="F9">
+        <v>3.8974797141610673E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.8948956731904981E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.57796015856992167</v>
+      </c>
+      <c r="C10">
+        <v>0.40386024372376028</v>
+      </c>
+      <c r="D10">
+        <v>0.3057265109464351</v>
+      </c>
+      <c r="E10">
+        <v>0.23740463622011421</v>
+      </c>
+      <c r="F10">
+        <v>0.19213212247778769</v>
+      </c>
+      <c r="G10">
+        <v>0.1647031798347865</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>0.1408097749756009</v>
+      </c>
+      <c r="C11">
+        <v>7.506164687743655E-2</v>
+      </c>
+      <c r="D11">
+        <v>4.9848421489331322E-2</v>
+      </c>
+      <c r="E11">
+        <v>2.827388925364344E-2</v>
+      </c>
+      <c r="F11">
+        <v>1.92763295113141E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.180792149726247E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.46438015810561939</v>
+      </c>
+      <c r="C12">
+        <v>0.29947066835284553</v>
+      </c>
+      <c r="D12">
+        <v>0.2059900308073275</v>
+      </c>
+      <c r="E12">
+        <v>0.13997649954224661</v>
+      </c>
+      <c r="F12">
+        <v>9.8680005825233869E-2</v>
+      </c>
+      <c r="G12">
+        <v>7.2896539286550405E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0.54454722325542637</v>
+      </c>
+      <c r="C13">
+        <v>0.3974189794287305</v>
+      </c>
+      <c r="D13">
+        <v>0.31183723450903972</v>
+      </c>
+      <c r="E13">
+        <v>0.25589168231084242</v>
+      </c>
+      <c r="F13">
+        <v>0.21597086338479049</v>
+      </c>
+      <c r="G13">
+        <v>0.18507869776337779</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1713,9 +2347,9 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +2372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1761,7 +2395,7 @@
         <v>0.22107418424811401</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +2418,7 @@
         <v>0.18864013164725671</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1807,7 +2441,7 @@
         <v>8.5640280182617504E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +2464,7 @@
         <v>1.0962365966432099E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1853,7 +2487,7 @@
         <v>0.1662040802351035</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1876,7 +2510,7 @@
         <v>1.4601671668094351E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1899,7 +2533,7 @@
         <v>1.44743156296438E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1922,7 +2556,7 @@
         <v>1.740419392436646E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1945,7 +2579,7 @@
         <v>6.6122577407550856E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1968,7 +2602,7 @@
         <v>0.1238725843155908</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1991,7 +2625,7 @@
         <v>0.10618661381878509</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2025,9 +2659,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2073,7 +2707,7 @@
         <v>0.14669469890471179</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2096,7 +2730,7 @@
         <v>0.208763355379497</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2119,7 +2753,7 @@
         <v>0.25017992075404732</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2776,7 @@
         <v>0.19284326920743861</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2165,7 +2799,7 @@
         <v>9.3574730829298416E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2188,7 +2822,7 @@
         <v>8.4669822929682188E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2211,7 +2845,7 @@
         <v>1.2932119073392419E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2868,7 @@
         <v>0.12758360976359701</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2257,7 +2891,7 @@
         <v>6.2961903577669773E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2280,7 +2914,7 @@
         <v>1.6963814900286759E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2303,7 +2937,7 @@
         <v>1.2473562931900609E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2337,9 +2971,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2362,7 +2996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2385,7 +3019,7 @@
         <v>0.1063071346484521</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2408,7 +3042,7 @@
         <v>0.15860534273332699</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +3065,7 @@
         <v>0.22188465296961779</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2454,7 +3088,7 @@
         <v>0.14539990381995019</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2477,7 +3111,7 @@
         <v>9.2433613252877633E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2500,7 +3134,7 @@
         <v>1.185703471830013E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +3157,7 @@
         <v>1.434135094113327E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2546,7 +3180,7 @@
         <v>9.7296912411288641E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2569,7 +3203,7 @@
         <v>7.4347373042242468E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2592,7 +3226,7 @@
         <v>1.9743668044320799E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2615,7 +3249,7 @@
         <v>1.7975724287899519E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2649,9 +3283,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2674,7 +3308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2697,7 +3331,7 @@
         <v>6.4364896659012932E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2720,7 +3354,7 @@
         <v>0.16883830438164729</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2743,7 +3377,7 @@
         <v>8.5726651340986948E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2766,7 +3400,7 @@
         <v>5.3203172337022563E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2789,7 +3423,7 @@
         <v>8.788164752938378E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2812,7 +3446,7 @@
         <v>4.8908863280010581E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2835,7 +3469,7 @@
         <v>3.1110554111237781E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2858,7 +3492,7 @@
         <v>6.047714105712123E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2881,7 +3515,7 @@
         <v>8.7406414598278317E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2904,7 +3538,7 @@
         <v>0.1175432274917947</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2927,7 +3561,7 @@
         <v>1.9905239167978921E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2961,9 +3595,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2986,7 +3620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3009,7 +3643,7 @@
         <v>9.8431748632955951E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3032,7 +3666,7 @@
         <v>0.19720190059873771</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3055,7 +3689,7 @@
         <v>0.19711592480824089</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3078,7 +3712,7 @@
         <v>6.205515659578708E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3101,7 +3735,7 @@
         <v>9.202634345271743E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3124,7 +3758,7 @@
         <v>4.5210427045479007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3147,7 +3781,7 @@
         <v>2.7970608233193341E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3170,7 +3804,7 @@
         <v>8.0141659615939526E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3193,7 +3827,7 @@
         <v>9.0385254450595129E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3216,7 +3850,7 @@
         <v>0.11322506215068349</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3239,7 +3873,7 @@
         <v>2.123317507392555E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3273,9 +3907,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3298,7 +3932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3321,7 +3955,7 @@
         <v>0.12598543622360381</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3344,7 +3978,7 @@
         <v>0.22398809344294829</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3367,7 +4001,7 @@
         <v>0.26200393282707768</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3390,7 +4024,7 @@
         <v>8.769232450365376E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3413,7 +4047,7 @@
         <v>0.1228312053983205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3436,7 +4070,7 @@
         <v>5.600072342713279E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3459,7 +4093,7 @@
         <v>3.7074776581050337E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3482,7 +4116,7 @@
         <v>9.3161526226595279E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3505,7 +4139,7 @@
         <v>9.2042539145534077E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3528,7 +4162,7 @@
         <v>9.7069166921206304E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3551,7 +4185,7 @@
         <v>2.8413379581771082E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3585,9 +4219,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3610,7 +4244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3633,7 +4267,7 @@
         <v>9.0677421873448197E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3656,7 +4290,7 @@
         <v>0.18564532718063939</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3679,7 +4313,7 @@
         <v>0.20427984848919831</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3702,7 +4336,7 @@
         <v>6.4636614049235014E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3725,7 +4359,7 @@
         <v>9.3029300625946276E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3748,7 +4382,7 @@
         <v>4.8350821361245577E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3771,7 +4405,7 @@
         <v>3.0539521790538891E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3794,7 +4428,7 @@
         <v>8.339434779849933E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3817,7 +4451,7 @@
         <v>0.1042477714866666</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3840,7 +4474,7 @@
         <v>0.11201277983126071</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3863,7 +4497,7 @@
         <v>2.2876836560715659E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3899,9 +4533,9 @@
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3924,7 +4558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3947,7 +4581,7 @@
         <v>6.7002638535033729E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3970,7 +4604,7 @@
         <v>7.7750884338902898E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3993,7 +4627,7 @@
         <v>4.5460779173834343E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4016,7 +4650,7 @@
         <v>6.8258077972422601E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -4039,7 +4673,7 @@
         <v>1.9320874579757969E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4062,7 +4696,7 @@
         <v>6.0182814811351293E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4085,7 +4719,7 @@
         <v>7.0571704114618605E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4108,7 +4742,7 @@
         <v>0.1021658779432687</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4131,7 +4765,7 @@
         <v>4.7675201910522033E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -4154,7 +4788,7 @@
         <v>2.9460959935557269E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -4177,7 +4811,7 @@
         <v>8.9785009060016033E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Modified and added more data and code
</commit_message>
<xml_diff>
--- a/Results/CSI_1_results.xlsx
+++ b/Results/CSI_1_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Geosciences_Project\Nowcasting_OF\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B202279-28B5-429D-A3D8-DBDA320A5A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91241494-5543-48D0-B5DD-44B88B270D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LK_persistence" sheetId="7" r:id="rId1"/>
@@ -25,15 +25,13 @@
     <sheet name="proesmans_extrapolation" sheetId="11" r:id="rId10"/>
     <sheet name="proesmans_sprog" sheetId="12" r:id="rId11"/>
     <sheet name="proesmans_anvil" sheetId="13" r:id="rId12"/>
-    <sheet name="VET_persistence" sheetId="14" r:id="rId13"/>
-    <sheet name="VET_extrapolation" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="19">
   <si>
     <t>Event</t>
   </si>
@@ -96,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,11 +107,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,12 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1715,630 +1705,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5727EB-4F5F-4BBA-AD38-0E35DB082C89}">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0.34847078528093761</v>
-      </c>
-      <c r="C2">
-        <v>0.20657729728399099</v>
-      </c>
-      <c r="D2">
-        <v>0.14283322642220889</v>
-      </c>
-      <c r="E2">
-        <v>0.10449376677107799</v>
-      </c>
-      <c r="F2">
-        <v>8.0780644502555149E-2</v>
-      </c>
-      <c r="G2">
-        <v>6.7002638535033729E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0.42973772801780902</v>
-      </c>
-      <c r="C3">
-        <v>0.267317091131477</v>
-      </c>
-      <c r="D3">
-        <v>0.19420543974774271</v>
-      </c>
-      <c r="E3">
-        <v>0.14615323284923931</v>
-      </c>
-      <c r="F3">
-        <v>0.10863080162755009</v>
-      </c>
-      <c r="G3">
-        <v>7.7750884338902898E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>7.3506261782311622E-2</v>
-      </c>
-      <c r="C4">
-        <v>4.116610517749255E-2</v>
-      </c>
-      <c r="D4">
-        <v>3.026140816005644E-2</v>
-      </c>
-      <c r="E4">
-        <v>2.697905299759264E-2</v>
-      </c>
-      <c r="F4">
-        <v>4.0935923285330751E-2</v>
-      </c>
-      <c r="G4">
-        <v>4.5460779173834343E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.40653954632564759</v>
-      </c>
-      <c r="C5">
-        <v>0.25934343340647331</v>
-      </c>
-      <c r="D5">
-        <v>0.1864329149978555</v>
-      </c>
-      <c r="E5">
-        <v>0.13548552225614749</v>
-      </c>
-      <c r="F5">
-        <v>9.6970336628080703E-2</v>
-      </c>
-      <c r="G5">
-        <v>6.8258077972422601E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>9.7807121511178097E-2</v>
-      </c>
-      <c r="C6">
-        <v>6.3358229707456887E-2</v>
-      </c>
-      <c r="D6">
-        <v>5.5416255175492632E-2</v>
-      </c>
-      <c r="E6">
-        <v>5.1360746133378751E-2</v>
-      </c>
-      <c r="F6">
-        <v>4.3632130485364892E-2</v>
-      </c>
-      <c r="G6">
-        <v>1.9320874579757969E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>0.47796097952526001</v>
-      </c>
-      <c r="C7">
-        <v>0.28524806061663133</v>
-      </c>
-      <c r="D7">
-        <v>0.18847598728427589</v>
-      </c>
-      <c r="E7">
-        <v>0.13118208993216729</v>
-      </c>
-      <c r="F7">
-        <v>8.9678030164244221E-2</v>
-      </c>
-      <c r="G7">
-        <v>6.0182814811351293E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.25306525044456413</v>
-      </c>
-      <c r="C8">
-        <v>0.16122256394848511</v>
-      </c>
-      <c r="D8">
-        <v>0.12636935219907469</v>
-      </c>
-      <c r="E8">
-        <v>9.7234758097743401E-2</v>
-      </c>
-      <c r="F8">
-        <v>9.1992835936770684E-2</v>
-      </c>
-      <c r="G8">
-        <v>7.0571704114618605E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>0.22571130028517769</v>
-      </c>
-      <c r="C9">
-        <v>0.10397584918959039</v>
-      </c>
-      <c r="D9">
-        <v>0.1012622835114096</v>
-      </c>
-      <c r="E9">
-        <v>0.1141565370792836</v>
-      </c>
-      <c r="F9">
-        <v>0.124133718072986</v>
-      </c>
-      <c r="G9">
-        <v>0.1021658779432687</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.39232696788164839</v>
-      </c>
-      <c r="C10">
-        <v>0.21706468613028129</v>
-      </c>
-      <c r="D10">
-        <v>0.13353450666139671</v>
-      </c>
-      <c r="E10">
-        <v>8.3044379565437976E-2</v>
-      </c>
-      <c r="F10">
-        <v>6.3112406247336911E-2</v>
-      </c>
-      <c r="G10">
-        <v>4.7675201910522033E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>6.013213258964837E-2</v>
-      </c>
-      <c r="C11">
-        <v>1.8439261400206991E-2</v>
-      </c>
-      <c r="D11">
-        <v>2.4585141814057219E-2</v>
-      </c>
-      <c r="E11">
-        <v>3.0108384011536211E-2</v>
-      </c>
-      <c r="F11">
-        <v>3.096864391086683E-2</v>
-      </c>
-      <c r="G11">
-        <v>2.9460959935557269E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>0.37260787625432867</v>
-      </c>
-      <c r="C12">
-        <v>0.24412611647619581</v>
-      </c>
-      <c r="D12">
-        <v>0.1701242340861836</v>
-      </c>
-      <c r="E12">
-        <v>0.1314104578169023</v>
-      </c>
-      <c r="F12">
-        <v>0.1077418318120619</v>
-      </c>
-      <c r="G12">
-        <v>8.9785009060016033E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>0.45207980570316991</v>
-      </c>
-      <c r="C13">
-        <v>0.30822964513480289</v>
-      </c>
-      <c r="D13">
-        <v>0.2381942629473624</v>
-      </c>
-      <c r="E13">
-        <v>0.19794567147584791</v>
-      </c>
-      <c r="F13">
-        <v>0.17471299677294741</v>
-      </c>
-      <c r="G13">
-        <v>0.15808902178187839</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92713F65-47E8-4579-8FB5-65F298BF647F}">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0.54305775985406668</v>
-      </c>
-      <c r="C2">
-        <v>0.37957508616374702</v>
-      </c>
-      <c r="D2">
-        <v>0.28796804287545841</v>
-      </c>
-      <c r="E2">
-        <v>0.22922923183821259</v>
-      </c>
-      <c r="F2">
-        <v>0.1869500041466215</v>
-      </c>
-      <c r="G2">
-        <v>0.15380936419628571</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0.64834896438464429</v>
-      </c>
-      <c r="C3">
-        <v>0.49934293669837881</v>
-      </c>
-      <c r="D3">
-        <v>0.40661988016707601</v>
-      </c>
-      <c r="E3">
-        <v>0.33760537887481329</v>
-      </c>
-      <c r="F3">
-        <v>0.27550397585578412</v>
-      </c>
-      <c r="G3">
-        <v>0.2210150843117773</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>5.4545188263365067E-2</v>
-      </c>
-      <c r="C4">
-        <v>1.8054905652850121E-2</v>
-      </c>
-      <c r="D4">
-        <v>1.2757172262503849E-2</v>
-      </c>
-      <c r="E4">
-        <v>8.7622217476931979E-3</v>
-      </c>
-      <c r="F4">
-        <v>1.266875486398447E-2</v>
-      </c>
-      <c r="G4">
-        <v>5.0548433379843669E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>0.55399305507806029</v>
-      </c>
-      <c r="C5">
-        <v>0.37286585385665738</v>
-      </c>
-      <c r="D5">
-        <v>0.26859426514967338</v>
-      </c>
-      <c r="E5">
-        <v>0.20508435560008889</v>
-      </c>
-      <c r="F5">
-        <v>0.16316414996814341</v>
-      </c>
-      <c r="G5">
-        <v>0.13349414280082211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>0.17955047596842921</v>
-      </c>
-      <c r="C6">
-        <v>8.1450247481258869E-2</v>
-      </c>
-      <c r="D6">
-        <v>3.7093858319336183E-2</v>
-      </c>
-      <c r="E6">
-        <v>2.0452783504902209E-2</v>
-      </c>
-      <c r="F6">
-        <v>7.4212324812973031E-3</v>
-      </c>
-      <c r="G6">
-        <v>9.5825532030025646E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>0.55423143957345822</v>
-      </c>
-      <c r="C7">
-        <v>0.35495217450879302</v>
-      </c>
-      <c r="D7">
-        <v>0.24771327833511661</v>
-      </c>
-      <c r="E7">
-        <v>0.1845702414959117</v>
-      </c>
-      <c r="F7">
-        <v>0.1412584282779879</v>
-      </c>
-      <c r="G7">
-        <v>0.10982556760443341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0.49009946341615801</v>
-      </c>
-      <c r="C8">
-        <v>0.32214717092039402</v>
-      </c>
-      <c r="D8">
-        <v>0.22669509264979809</v>
-      </c>
-      <c r="E8">
-        <v>0.16158330651940311</v>
-      </c>
-      <c r="F8">
-        <v>0.1197440860151482</v>
-      </c>
-      <c r="G8">
-        <v>8.8538936683520156E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>0.40460576621925071</v>
-      </c>
-      <c r="C9">
-        <v>0.2241751017540399</v>
-      </c>
-      <c r="D9">
-        <v>0.1213529991790033</v>
-      </c>
-      <c r="E9">
-        <v>6.8198268881454277E-2</v>
-      </c>
-      <c r="F9">
-        <v>3.8974797141610673E-2</v>
-      </c>
-      <c r="G9">
-        <v>1.8948956731904981E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.57796015856992167</v>
-      </c>
-      <c r="C10">
-        <v>0.40386024372376028</v>
-      </c>
-      <c r="D10">
-        <v>0.3057265109464351</v>
-      </c>
-      <c r="E10">
-        <v>0.23740463622011421</v>
-      </c>
-      <c r="F10">
-        <v>0.19213212247778769</v>
-      </c>
-      <c r="G10">
-        <v>0.1647031798347865</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>0.1408097749756009</v>
-      </c>
-      <c r="C11">
-        <v>7.506164687743655E-2</v>
-      </c>
-      <c r="D11">
-        <v>4.9848421489331322E-2</v>
-      </c>
-      <c r="E11">
-        <v>2.827388925364344E-2</v>
-      </c>
-      <c r="F11">
-        <v>1.92763295113141E-2</v>
-      </c>
-      <c r="G11">
-        <v>1.180792149726247E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>0.46438015810561939</v>
-      </c>
-      <c r="C12">
-        <v>0.29947066835284553</v>
-      </c>
-      <c r="D12">
-        <v>0.2059900308073275</v>
-      </c>
-      <c r="E12">
-        <v>0.13997649954224661</v>
-      </c>
-      <c r="F12">
-        <v>9.8680005825233869E-2</v>
-      </c>
-      <c r="G12">
-        <v>7.2896539286550405E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>0.54454722325542637</v>
-      </c>
-      <c r="C13">
-        <v>0.3974189794287305</v>
-      </c>
-      <c r="D13">
-        <v>0.31183723450903972</v>
-      </c>
-      <c r="E13">
-        <v>0.25589168231084242</v>
-      </c>
-      <c r="F13">
-        <v>0.21597086338479049</v>
-      </c>
-      <c r="G13">
-        <v>0.18507869776337779</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380EF224-004F-EB49-A7DD-B149832C64BE}">
   <dimension ref="A1:G13"/>

</xml_diff>